<commit_message>
Added an empty line and changed example.xlsx
</commit_message>
<xml_diff>
--- a/bin/example.xlsx
+++ b/bin/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konrad\Documents\IT\python\GIS_Downloader\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550E6D48-AC49-4CE3-8C94-591A5385CD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4916E9-968D-425A-976F-F10E7CEB7940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-810" windowWidth="29040" windowHeight="15840" xr2:uid="{58524872-B396-42E0-8C80-5390EC9F6C07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58524872-B396-42E0-8C80-5390EC9F6C07}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -459,7 +459,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>